<commit_message>
update of main management scripts
</commit_message>
<xml_diff>
--- a/utils/scripts/template_insert_insegnamenti.xlsx
+++ b/utils/scripts/template_insert_insegnamenti.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t xml:space="preserve">Cognome</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
+    <t xml:space="preserve">NOTE:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mancuso</t>
   </si>
   <si>
@@ -73,6 +76,12 @@
     <t xml:space="preserve">Sistemi e Reti</t>
   </si>
   <si>
+    <t xml:space="preserve">LISTA DELLE MATERIE VALIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTA DELLE SEZIONI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moretti</t>
   </si>
   <si>
@@ -94,6 +103,12 @@
     <t xml:space="preserve">Inglese</t>
   </si>
   <si>
+    <t xml:space="preserve">Biologia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ghio</t>
   </si>
   <si>
@@ -103,7 +118,136 @@
     <t xml:space="preserve">IV</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
+    <t xml:space="preserve">CLIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chimica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diritto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MECC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disegno e Arte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educazione Civica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elettronica ed Elettrotecnica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filosofia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geografia Economica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geography IGCSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geostoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impianti Laboratorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inglese Gruppo A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inglese Gruppo B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inglese Gruppo C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matematica e Complementi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mathematics IGCSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meccanica e Macchine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Religione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA Elettronica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA Energia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA Informatica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA Meccatronica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scienze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scienze Motorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scienze della Terra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistemi Elettronici</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistemi e Automazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaking Madrelingua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPSEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnologia Laboratorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnologia Meccanica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnologie e Tecniche di Rappresentazione Grafiche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telecomunicazioni</t>
   </si>
 </sst>
 </file>
@@ -205,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,6 +364,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -349,17 +501,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H236"/>
+  <dimension ref="A1:M236"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,13 +565,16 @@
       <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>2024</v>
@@ -442,10 +597,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>2024</v>
@@ -465,25 +620,33 @@
       <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="J4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>2024</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>13</v>
@@ -494,10 +657,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>2024</v>
@@ -517,31 +680,43 @@
       <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>2024</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,6 +728,12 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
+      <c r="J8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -563,6 +744,12 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
+      <c r="J9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -573,6 +760,12 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
+      <c r="J10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -583,6 +776,12 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
+      <c r="J11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -593,6 +792,12 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
+      <c r="J12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
@@ -603,402 +808,522 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="J13" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
+      <c r="J14" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
+      <c r="J15" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
+      <c r="J16" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
+      <c r="J17" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
+      <c r="J18" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
+      <c r="J19" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
+      <c r="J20" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
+      <c r="J21" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
+      <c r="J22" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
+      <c r="J23" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
+      <c r="J24" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
+      <c r="J25" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
+      <c r="J26" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
+      <c r="J27" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
+      <c r="J28" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
+      <c r="J29" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
+      <c r="J30" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
+      <c r="J31" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="6"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
+      <c r="J32" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="6"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
+      <c r="J33" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="6"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
+      <c r="J34" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="6"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
+      <c r="J35" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
+      <c r="D36" s="6"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
+      <c r="J36" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
+      <c r="J37" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
+      <c r="J38" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
+      <c r="D39" s="6"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
+      <c r="J39" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
+      <c r="D40" s="6"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
+      <c r="J40" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="6"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
+      <c r="J41" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="6"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
+      <c r="J42" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
+      <c r="D43" s="6"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
+      <c r="J43" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="4"/>
+      <c r="D44" s="6"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
+      <c r="J44" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
+      <c r="D45" s="6"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
+      <c r="J45" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="4"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
+      <c r="J46" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
+      <c r="D47" s="6"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
+      <c r="J47" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="4"/>
+      <c r="D48" s="6"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
+      <c r="J48" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="4"/>
+      <c r="D49" s="6"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
+      <c r="J49" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="4"/>
+      <c r="D50" s="6"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
+      <c r="J50" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="4"/>
+      <c r="D51" s="6"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
+      <c r="J51" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="4"/>
+      <c r="D52" s="6"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
+      <c r="J52" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="4"/>
+      <c r="D53" s="6"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -1008,7 +1333,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="4"/>
+      <c r="D54" s="6"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -1018,7 +1343,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="4"/>
+      <c r="D55" s="6"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -1028,7 +1353,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="4"/>
+      <c r="D56" s="6"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -1038,7 +1363,7 @@
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="4"/>
+      <c r="D57" s="6"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -1048,7 +1373,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="4"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -1058,7 +1383,7 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="4"/>
+      <c r="D59" s="6"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -1068,7 +1393,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="4"/>
+      <c r="D60" s="6"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -1078,7 +1403,7 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="4"/>
+      <c r="D61" s="6"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -1088,7 +1413,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="4"/>
+      <c r="D62" s="6"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -1098,7 +1423,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="4"/>
+      <c r="D63" s="6"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -1108,7 +1433,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="4"/>
+      <c r="D64" s="6"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -1118,7 +1443,7 @@
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="4"/>
+      <c r="D65" s="6"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -1128,7 +1453,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="4"/>
+      <c r="D66" s="6"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -1138,7 +1463,7 @@
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
+      <c r="D67" s="6"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -1148,7 +1473,7 @@
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="4"/>
+      <c r="D68" s="6"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -1158,7 +1483,7 @@
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="4"/>
+      <c r="D69" s="6"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -1168,7 +1493,7 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="4"/>
+      <c r="D70" s="6"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -1178,7 +1503,7 @@
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="4"/>
+      <c r="D71" s="6"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -1188,7 +1513,7 @@
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="4"/>
+      <c r="D72" s="6"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -1198,7 +1523,7 @@
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="6"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -1208,7 +1533,7 @@
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="4"/>
+      <c r="D74" s="6"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -1218,7 +1543,7 @@
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="4"/>
+      <c r="D75" s="6"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -1228,7 +1553,7 @@
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="4"/>
+      <c r="D76" s="6"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -1238,7 +1563,7 @@
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="4"/>
+      <c r="D77" s="6"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -1248,7 +1573,7 @@
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="4"/>
+      <c r="D78" s="6"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -1258,7 +1583,7 @@
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="4"/>
+      <c r="D79" s="6"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -1268,7 +1593,7 @@
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="4"/>
+      <c r="D80" s="6"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -1278,7 +1603,7 @@
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="4"/>
+      <c r="D81" s="6"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -1288,7 +1613,7 @@
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="4"/>
+      <c r="D82" s="6"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -1298,7 +1623,7 @@
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="4"/>
+      <c r="D83" s="6"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -1308,7 +1633,7 @@
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="4"/>
+      <c r="D84" s="6"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -1318,7 +1643,7 @@
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
-      <c r="D85" s="4"/>
+      <c r="D85" s="6"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -1328,7 +1653,7 @@
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="4"/>
+      <c r="D86" s="6"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -1338,7 +1663,7 @@
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
-      <c r="D87" s="4"/>
+      <c r="D87" s="6"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -1348,7 +1673,7 @@
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
-      <c r="D88" s="4"/>
+      <c r="D88" s="6"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -1358,7 +1683,7 @@
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
-      <c r="D89" s="4"/>
+      <c r="D89" s="6"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -1368,7 +1693,7 @@
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="4"/>
+      <c r="D90" s="6"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -1378,7 +1703,7 @@
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
-      <c r="D91" s="4"/>
+      <c r="D91" s="6"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -1388,7 +1713,7 @@
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
-      <c r="D92" s="4"/>
+      <c r="D92" s="6"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -1398,7 +1723,7 @@
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
-      <c r="D93" s="4"/>
+      <c r="D93" s="6"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -1408,7 +1733,7 @@
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="4"/>
+      <c r="D94" s="6"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -1418,7 +1743,7 @@
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="4"/>
+      <c r="D95" s="6"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -1428,7 +1753,7 @@
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
-      <c r="D96" s="4"/>
+      <c r="D96" s="6"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -1438,7 +1763,7 @@
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
-      <c r="D97" s="4"/>
+      <c r="D97" s="6"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -1448,7 +1773,7 @@
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="4"/>
+      <c r="D98" s="6"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -1458,7 +1783,7 @@
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
-      <c r="D99" s="4"/>
+      <c r="D99" s="6"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -1468,7 +1793,7 @@
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
-      <c r="D100" s="4"/>
+      <c r="D100" s="6"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
@@ -1478,7 +1803,7 @@
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
-      <c r="D101" s="4"/>
+      <c r="D101" s="6"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -1488,7 +1813,7 @@
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
-      <c r="D102" s="4"/>
+      <c r="D102" s="6"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
@@ -1498,7 +1823,7 @@
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
-      <c r="D103" s="4"/>
+      <c r="D103" s="6"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
@@ -1508,7 +1833,7 @@
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
-      <c r="D104" s="4"/>
+      <c r="D104" s="6"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -1518,7 +1843,7 @@
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
-      <c r="D105" s="4"/>
+      <c r="D105" s="6"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -1528,7 +1853,7 @@
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
-      <c r="D106" s="4"/>
+      <c r="D106" s="6"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -1538,7 +1863,7 @@
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
-      <c r="D107" s="4"/>
+      <c r="D107" s="6"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -1548,7 +1873,7 @@
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
-      <c r="D108" s="4"/>
+      <c r="D108" s="6"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
@@ -1558,7 +1883,7 @@
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
-      <c r="D109" s="4"/>
+      <c r="D109" s="6"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -1568,7 +1893,7 @@
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
-      <c r="D110" s="4"/>
+      <c r="D110" s="6"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -1578,7 +1903,7 @@
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
-      <c r="D111" s="4"/>
+      <c r="D111" s="6"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
@@ -1588,7 +1913,7 @@
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
-      <c r="D112" s="4"/>
+      <c r="D112" s="6"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -1598,7 +1923,7 @@
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
-      <c r="D113" s="4"/>
+      <c r="D113" s="6"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -1608,7 +1933,7 @@
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
-      <c r="D114" s="4"/>
+      <c r="D114" s="6"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -1618,7 +1943,7 @@
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
-      <c r="D115" s="4"/>
+      <c r="D115" s="6"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
@@ -1628,7 +1953,7 @@
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
-      <c r="D116" s="4"/>
+      <c r="D116" s="6"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
@@ -1638,7 +1963,7 @@
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
-      <c r="D117" s="4"/>
+      <c r="D117" s="6"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
@@ -1648,7 +1973,7 @@
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
-      <c r="D118" s="4"/>
+      <c r="D118" s="6"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -1658,7 +1983,7 @@
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
-      <c r="D119" s="4"/>
+      <c r="D119" s="6"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
@@ -1668,7 +1993,7 @@
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
-      <c r="D120" s="4"/>
+      <c r="D120" s="6"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
@@ -1678,7 +2003,7 @@
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
-      <c r="D121" s="4"/>
+      <c r="D121" s="6"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -1688,7 +2013,7 @@
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
-      <c r="D122" s="4"/>
+      <c r="D122" s="6"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -1698,7 +2023,7 @@
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
-      <c r="D123" s="4"/>
+      <c r="D123" s="6"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
@@ -1708,7 +2033,7 @@
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
-      <c r="D124" s="4"/>
+      <c r="D124" s="6"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -1718,7 +2043,7 @@
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
-      <c r="D125" s="4"/>
+      <c r="D125" s="6"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -1728,7 +2053,7 @@
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
-      <c r="D126" s="4"/>
+      <c r="D126" s="6"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
@@ -1738,7 +2063,7 @@
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
-      <c r="D127" s="4"/>
+      <c r="D127" s="6"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
@@ -1748,7 +2073,7 @@
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
-      <c r="D128" s="4"/>
+      <c r="D128" s="6"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
@@ -1758,7 +2083,7 @@
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
-      <c r="D129" s="4"/>
+      <c r="D129" s="6"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -1768,7 +2093,7 @@
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
-      <c r="D130" s="4"/>
+      <c r="D130" s="6"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
@@ -1778,7 +2103,7 @@
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
-      <c r="D131" s="4"/>
+      <c r="D131" s="6"/>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
@@ -1788,7 +2113,7 @@
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
-      <c r="D132" s="4"/>
+      <c r="D132" s="6"/>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
@@ -1798,7 +2123,7 @@
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
-      <c r="D133" s="4"/>
+      <c r="D133" s="6"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
@@ -1808,7 +2133,7 @@
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
-      <c r="D134" s="4"/>
+      <c r="D134" s="6"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
@@ -1818,7 +2143,7 @@
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
-      <c r="D135" s="4"/>
+      <c r="D135" s="6"/>
       <c r="E135" s="3"/>
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
@@ -1828,7 +2153,7 @@
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
-      <c r="D136" s="4"/>
+      <c r="D136" s="6"/>
       <c r="E136" s="3"/>
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
@@ -1838,7 +2163,7 @@
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
-      <c r="D137" s="4"/>
+      <c r="D137" s="6"/>
       <c r="E137" s="3"/>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
@@ -1848,7 +2173,7 @@
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
-      <c r="D138" s="4"/>
+      <c r="D138" s="6"/>
       <c r="E138" s="3"/>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
@@ -1858,7 +2183,7 @@
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
-      <c r="D139" s="4"/>
+      <c r="D139" s="6"/>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
       <c r="G139" s="3"/>
@@ -1868,7 +2193,7 @@
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
-      <c r="D140" s="4"/>
+      <c r="D140" s="6"/>
       <c r="E140" s="3"/>
       <c r="F140" s="3"/>
       <c r="G140" s="3"/>
@@ -1878,7 +2203,7 @@
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
-      <c r="D141" s="4"/>
+      <c r="D141" s="6"/>
       <c r="E141" s="3"/>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -1888,7 +2213,7 @@
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
-      <c r="D142" s="4"/>
+      <c r="D142" s="6"/>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
@@ -1898,7 +2223,7 @@
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
-      <c r="D143" s="4"/>
+      <c r="D143" s="6"/>
       <c r="E143" s="3"/>
       <c r="F143" s="3"/>
       <c r="G143" s="3"/>
@@ -1908,7 +2233,7 @@
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
-      <c r="D144" s="4"/>
+      <c r="D144" s="6"/>
       <c r="E144" s="3"/>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
@@ -1918,7 +2243,7 @@
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
-      <c r="D145" s="4"/>
+      <c r="D145" s="6"/>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
@@ -1928,7 +2253,7 @@
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
-      <c r="D146" s="4"/>
+      <c r="D146" s="6"/>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
       <c r="G146" s="3"/>
@@ -1938,7 +2263,7 @@
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
-      <c r="D147" s="4"/>
+      <c r="D147" s="6"/>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
@@ -1948,7 +2273,7 @@
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
-      <c r="D148" s="4"/>
+      <c r="D148" s="6"/>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
       <c r="G148" s="3"/>
@@ -1958,7 +2283,7 @@
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
-      <c r="D149" s="4"/>
+      <c r="D149" s="6"/>
       <c r="E149" s="3"/>
       <c r="F149" s="3"/>
       <c r="G149" s="3"/>
@@ -1968,7 +2293,7 @@
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
-      <c r="D150" s="4"/>
+      <c r="D150" s="6"/>
       <c r="E150" s="3"/>
       <c r="F150" s="3"/>
       <c r="G150" s="3"/>
@@ -1978,7 +2303,7 @@
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
-      <c r="D151" s="4"/>
+      <c r="D151" s="6"/>
       <c r="E151" s="3"/>
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
@@ -1988,7 +2313,7 @@
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
-      <c r="D152" s="4"/>
+      <c r="D152" s="6"/>
       <c r="E152" s="3"/>
       <c r="F152" s="3"/>
       <c r="G152" s="3"/>
@@ -1998,7 +2323,7 @@
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
-      <c r="D153" s="4"/>
+      <c r="D153" s="6"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
@@ -2008,7 +2333,7 @@
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
-      <c r="D154" s="4"/>
+      <c r="D154" s="6"/>
       <c r="E154" s="3"/>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -2018,7 +2343,7 @@
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
-      <c r="D155" s="4"/>
+      <c r="D155" s="6"/>
       <c r="E155" s="3"/>
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
@@ -2028,7 +2353,7 @@
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
-      <c r="D156" s="4"/>
+      <c r="D156" s="6"/>
       <c r="E156" s="3"/>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
@@ -2038,7 +2363,7 @@
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
-      <c r="D157" s="4"/>
+      <c r="D157" s="6"/>
       <c r="E157" s="3"/>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
@@ -2048,7 +2373,7 @@
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
-      <c r="D158" s="4"/>
+      <c r="D158" s="6"/>
       <c r="E158" s="3"/>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
@@ -2058,7 +2383,7 @@
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
-      <c r="D159" s="4"/>
+      <c r="D159" s="6"/>
       <c r="E159" s="3"/>
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
@@ -2068,7 +2393,7 @@
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
-      <c r="D160" s="4"/>
+      <c r="D160" s="6"/>
       <c r="E160" s="3"/>
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
@@ -2078,7 +2403,7 @@
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
-      <c r="D161" s="4"/>
+      <c r="D161" s="6"/>
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
@@ -2088,7 +2413,7 @@
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
-      <c r="D162" s="4"/>
+      <c r="D162" s="6"/>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
       <c r="G162" s="3"/>
@@ -2098,7 +2423,7 @@
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
-      <c r="D163" s="4"/>
+      <c r="D163" s="6"/>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
       <c r="G163" s="3"/>
@@ -2108,7 +2433,7 @@
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
-      <c r="D164" s="4"/>
+      <c r="D164" s="6"/>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
@@ -2118,7 +2443,7 @@
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
-      <c r="D165" s="4"/>
+      <c r="D165" s="6"/>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
@@ -2128,7 +2453,7 @@
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
-      <c r="D166" s="4"/>
+      <c r="D166" s="6"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
       <c r="G166" s="3"/>
@@ -2138,7 +2463,7 @@
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
-      <c r="D167" s="4"/>
+      <c r="D167" s="6"/>
       <c r="E167" s="3"/>
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
@@ -2148,7 +2473,7 @@
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
-      <c r="D168" s="4"/>
+      <c r="D168" s="6"/>
       <c r="E168" s="3"/>
       <c r="F168" s="3"/>
       <c r="G168" s="3"/>
@@ -2158,7 +2483,7 @@
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
-      <c r="D169" s="4"/>
+      <c r="D169" s="6"/>
       <c r="E169" s="3"/>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
@@ -2168,7 +2493,7 @@
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
-      <c r="D170" s="4"/>
+      <c r="D170" s="6"/>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
@@ -2178,7 +2503,7 @@
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
-      <c r="D171" s="4"/>
+      <c r="D171" s="6"/>
       <c r="E171" s="3"/>
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
@@ -2188,7 +2513,7 @@
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
-      <c r="D172" s="4"/>
+      <c r="D172" s="6"/>
       <c r="E172" s="3"/>
       <c r="F172" s="3"/>
       <c r="G172" s="3"/>
@@ -2198,7 +2523,7 @@
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
-      <c r="D173" s="4"/>
+      <c r="D173" s="6"/>
       <c r="E173" s="3"/>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
@@ -2208,7 +2533,7 @@
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
-      <c r="D174" s="4"/>
+      <c r="D174" s="6"/>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -2218,7 +2543,7 @@
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
-      <c r="D175" s="4"/>
+      <c r="D175" s="6"/>
       <c r="E175" s="3"/>
       <c r="F175" s="3"/>
       <c r="G175" s="3"/>
@@ -2228,7 +2553,7 @@
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
-      <c r="D176" s="4"/>
+      <c r="D176" s="6"/>
       <c r="E176" s="3"/>
       <c r="F176" s="3"/>
       <c r="G176" s="3"/>
@@ -2238,7 +2563,7 @@
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
-      <c r="D177" s="4"/>
+      <c r="D177" s="6"/>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
@@ -2248,7 +2573,7 @@
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
-      <c r="D178" s="4"/>
+      <c r="D178" s="6"/>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
       <c r="G178" s="3"/>
@@ -2258,7 +2583,7 @@
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
-      <c r="D179" s="4"/>
+      <c r="D179" s="6"/>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
       <c r="G179" s="3"/>
@@ -2268,7 +2593,7 @@
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
-      <c r="D180" s="4"/>
+      <c r="D180" s="6"/>
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
@@ -2278,7 +2603,7 @@
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
-      <c r="D181" s="4"/>
+      <c r="D181" s="6"/>
       <c r="E181" s="3"/>
       <c r="F181" s="3"/>
       <c r="G181" s="3"/>
@@ -2288,7 +2613,7 @@
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
-      <c r="D182" s="4"/>
+      <c r="D182" s="6"/>
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
       <c r="G182" s="3"/>
@@ -2298,7 +2623,7 @@
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
-      <c r="D183" s="4"/>
+      <c r="D183" s="6"/>
       <c r="E183" s="3"/>
       <c r="F183" s="3"/>
       <c r="G183" s="3"/>
@@ -2308,7 +2633,7 @@
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
-      <c r="D184" s="4"/>
+      <c r="D184" s="6"/>
       <c r="E184" s="3"/>
       <c r="F184" s="3"/>
       <c r="G184" s="3"/>
@@ -2318,7 +2643,7 @@
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
-      <c r="D185" s="4"/>
+      <c r="D185" s="6"/>
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
@@ -2328,7 +2653,7 @@
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
-      <c r="D186" s="4"/>
+      <c r="D186" s="6"/>
       <c r="E186" s="3"/>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -2338,7 +2663,7 @@
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
-      <c r="D187" s="4"/>
+      <c r="D187" s="6"/>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
@@ -2348,7 +2673,7 @@
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
-      <c r="D188" s="4"/>
+      <c r="D188" s="6"/>
       <c r="E188" s="3"/>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -2358,7 +2683,7 @@
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
-      <c r="D189" s="4"/>
+      <c r="D189" s="6"/>
       <c r="E189" s="3"/>
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
@@ -2368,7 +2693,7 @@
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
-      <c r="D190" s="4"/>
+      <c r="D190" s="6"/>
       <c r="E190" s="3"/>
       <c r="F190" s="3"/>
       <c r="G190" s="3"/>
@@ -2378,7 +2703,7 @@
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
-      <c r="D191" s="4"/>
+      <c r="D191" s="6"/>
       <c r="E191" s="3"/>
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
@@ -2388,7 +2713,7 @@
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
-      <c r="D192" s="4"/>
+      <c r="D192" s="6"/>
       <c r="E192" s="3"/>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
@@ -2398,7 +2723,7 @@
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
-      <c r="D193" s="4"/>
+      <c r="D193" s="6"/>
       <c r="E193" s="3"/>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
@@ -2408,7 +2733,7 @@
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
-      <c r="D194" s="4"/>
+      <c r="D194" s="6"/>
       <c r="E194" s="3"/>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
@@ -2418,7 +2743,7 @@
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
-      <c r="D195" s="4"/>
+      <c r="D195" s="6"/>
       <c r="E195" s="3"/>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
@@ -2428,7 +2753,7 @@
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
-      <c r="D196" s="4"/>
+      <c r="D196" s="6"/>
       <c r="E196" s="3"/>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
@@ -2438,7 +2763,7 @@
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
-      <c r="D197" s="4"/>
+      <c r="D197" s="6"/>
       <c r="E197" s="3"/>
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
@@ -2448,7 +2773,7 @@
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
-      <c r="D198" s="4"/>
+      <c r="D198" s="6"/>
       <c r="E198" s="3"/>
       <c r="F198" s="3"/>
       <c r="G198" s="3"/>
@@ -2458,7 +2783,7 @@
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
-      <c r="D199" s="4"/>
+      <c r="D199" s="6"/>
       <c r="E199" s="3"/>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
@@ -2468,7 +2793,7 @@
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
-      <c r="D200" s="4"/>
+      <c r="D200" s="6"/>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
       <c r="G200" s="3"/>
@@ -2478,7 +2803,7 @@
       <c r="A201" s="3"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
-      <c r="D201" s="4"/>
+      <c r="D201" s="6"/>
       <c r="E201" s="3"/>
       <c r="F201" s="3"/>
       <c r="G201" s="3"/>
@@ -2488,7 +2813,7 @@
       <c r="A202" s="3"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
-      <c r="D202" s="4"/>
+      <c r="D202" s="6"/>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
       <c r="G202" s="3"/>
@@ -2498,7 +2823,7 @@
       <c r="A203" s="3"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
-      <c r="D203" s="4"/>
+      <c r="D203" s="6"/>
       <c r="E203" s="3"/>
       <c r="F203" s="3"/>
       <c r="G203" s="3"/>
@@ -2508,7 +2833,7 @@
       <c r="A204" s="3"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
-      <c r="D204" s="4"/>
+      <c r="D204" s="6"/>
       <c r="E204" s="3"/>
       <c r="F204" s="3"/>
       <c r="G204" s="3"/>
@@ -2518,7 +2843,7 @@
       <c r="A205" s="3"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
-      <c r="D205" s="4"/>
+      <c r="D205" s="6"/>
       <c r="E205" s="3"/>
       <c r="F205" s="3"/>
       <c r="G205" s="3"/>
@@ -2528,7 +2853,7 @@
       <c r="A206" s="3"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
-      <c r="D206" s="4"/>
+      <c r="D206" s="6"/>
       <c r="E206" s="3"/>
       <c r="F206" s="3"/>
       <c r="G206" s="3"/>
@@ -2538,7 +2863,7 @@
       <c r="A207" s="3"/>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
-      <c r="D207" s="4"/>
+      <c r="D207" s="6"/>
       <c r="E207" s="3"/>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
@@ -2548,7 +2873,7 @@
       <c r="A208" s="3"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
-      <c r="D208" s="4"/>
+      <c r="D208" s="6"/>
       <c r="E208" s="3"/>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
@@ -2558,7 +2883,7 @@
       <c r="A209" s="3"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
-      <c r="D209" s="4"/>
+      <c r="D209" s="6"/>
       <c r="E209" s="3"/>
       <c r="F209" s="3"/>
       <c r="G209" s="3"/>
@@ -2568,7 +2893,7 @@
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
-      <c r="D210" s="4"/>
+      <c r="D210" s="6"/>
       <c r="E210" s="3"/>
       <c r="F210" s="3"/>
       <c r="G210" s="3"/>
@@ -2578,7 +2903,7 @@
       <c r="A211" s="3"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
-      <c r="D211" s="4"/>
+      <c r="D211" s="6"/>
       <c r="E211" s="3"/>
       <c r="F211" s="3"/>
       <c r="G211" s="3"/>
@@ -2588,7 +2913,7 @@
       <c r="A212" s="3"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
-      <c r="D212" s="4"/>
+      <c r="D212" s="6"/>
       <c r="E212" s="3"/>
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
@@ -2598,7 +2923,7 @@
       <c r="A213" s="3"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
-      <c r="D213" s="4"/>
+      <c r="D213" s="6"/>
       <c r="E213" s="3"/>
       <c r="F213" s="3"/>
       <c r="G213" s="3"/>
@@ -2608,7 +2933,7 @@
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
-      <c r="D214" s="4"/>
+      <c r="D214" s="6"/>
       <c r="E214" s="3"/>
       <c r="F214" s="3"/>
       <c r="G214" s="3"/>
@@ -2618,7 +2943,7 @@
       <c r="A215" s="3"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
-      <c r="D215" s="4"/>
+      <c r="D215" s="6"/>
       <c r="E215" s="3"/>
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
@@ -2628,7 +2953,7 @@
       <c r="A216" s="3"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
-      <c r="D216" s="4"/>
+      <c r="D216" s="6"/>
       <c r="E216" s="3"/>
       <c r="F216" s="3"/>
       <c r="G216" s="3"/>
@@ -2638,7 +2963,7 @@
       <c r="A217" s="3"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
-      <c r="D217" s="4"/>
+      <c r="D217" s="6"/>
       <c r="E217" s="3"/>
       <c r="F217" s="3"/>
       <c r="G217" s="3"/>
@@ -2648,7 +2973,7 @@
       <c r="A218" s="3"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
-      <c r="D218" s="4"/>
+      <c r="D218" s="6"/>
       <c r="E218" s="3"/>
       <c r="F218" s="3"/>
       <c r="G218" s="3"/>
@@ -2658,7 +2983,7 @@
       <c r="A219" s="3"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
-      <c r="D219" s="4"/>
+      <c r="D219" s="6"/>
       <c r="E219" s="3"/>
       <c r="F219" s="3"/>
       <c r="G219" s="3"/>
@@ -2668,7 +2993,7 @@
       <c r="A220" s="3"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
-      <c r="D220" s="4"/>
+      <c r="D220" s="6"/>
       <c r="E220" s="3"/>
       <c r="F220" s="3"/>
       <c r="G220" s="3"/>
@@ -2678,7 +3003,7 @@
       <c r="A221" s="3"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
-      <c r="D221" s="4"/>
+      <c r="D221" s="6"/>
       <c r="E221" s="3"/>
       <c r="F221" s="3"/>
       <c r="G221" s="3"/>
@@ -2688,7 +3013,7 @@
       <c r="A222" s="3"/>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
-      <c r="D222" s="4"/>
+      <c r="D222" s="6"/>
       <c r="E222" s="3"/>
       <c r="F222" s="3"/>
       <c r="G222" s="3"/>
@@ -2698,7 +3023,7 @@
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
-      <c r="D223" s="4"/>
+      <c r="D223" s="6"/>
       <c r="E223" s="3"/>
       <c r="F223" s="3"/>
       <c r="G223" s="3"/>
@@ -2708,7 +3033,7 @@
       <c r="A224" s="3"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
-      <c r="D224" s="4"/>
+      <c r="D224" s="6"/>
       <c r="E224" s="3"/>
       <c r="F224" s="3"/>
       <c r="G224" s="3"/>
@@ -2718,7 +3043,7 @@
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
-      <c r="D225" s="4"/>
+      <c r="D225" s="6"/>
       <c r="E225" s="3"/>
       <c r="F225" s="3"/>
       <c r="G225" s="3"/>
@@ -2728,7 +3053,7 @@
       <c r="A226" s="3"/>
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
-      <c r="D226" s="4"/>
+      <c r="D226" s="6"/>
       <c r="E226" s="3"/>
       <c r="F226" s="3"/>
       <c r="G226" s="3"/>
@@ -2738,7 +3063,7 @@
       <c r="A227" s="3"/>
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
-      <c r="D227" s="4"/>
+      <c r="D227" s="6"/>
       <c r="E227" s="3"/>
       <c r="F227" s="3"/>
       <c r="G227" s="3"/>
@@ -2748,7 +3073,7 @@
       <c r="A228" s="3"/>
       <c r="B228" s="3"/>
       <c r="C228" s="3"/>
-      <c r="D228" s="4"/>
+      <c r="D228" s="6"/>
       <c r="E228" s="3"/>
       <c r="F228" s="3"/>
       <c r="G228" s="3"/>
@@ -2758,7 +3083,7 @@
       <c r="A229" s="3"/>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
-      <c r="D229" s="4"/>
+      <c r="D229" s="6"/>
       <c r="E229" s="3"/>
       <c r="F229" s="3"/>
       <c r="G229" s="3"/>
@@ -2768,7 +3093,7 @@
       <c r="A230" s="3"/>
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
-      <c r="D230" s="4"/>
+      <c r="D230" s="6"/>
       <c r="E230" s="3"/>
       <c r="F230" s="3"/>
       <c r="G230" s="3"/>
@@ -2778,7 +3103,7 @@
       <c r="A231" s="3"/>
       <c r="B231" s="3"/>
       <c r="C231" s="3"/>
-      <c r="D231" s="4"/>
+      <c r="D231" s="6"/>
       <c r="E231" s="3"/>
       <c r="F231" s="3"/>
       <c r="G231" s="3"/>
@@ -2788,7 +3113,7 @@
       <c r="A232" s="3"/>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
-      <c r="D232" s="4"/>
+      <c r="D232" s="6"/>
       <c r="E232" s="3"/>
       <c r="F232" s="3"/>
       <c r="G232" s="3"/>
@@ -2798,7 +3123,7 @@
       <c r="A233" s="3"/>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
-      <c r="D233" s="4"/>
+      <c r="D233" s="6"/>
       <c r="E233" s="3"/>
       <c r="F233" s="3"/>
       <c r="G233" s="3"/>
@@ -2808,7 +3133,7 @@
       <c r="A234" s="3"/>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
-      <c r="D234" s="4"/>
+      <c r="D234" s="6"/>
       <c r="E234" s="3"/>
       <c r="F234" s="3"/>
       <c r="G234" s="3"/>
@@ -2818,7 +3143,7 @@
       <c r="A235" s="3"/>
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
-      <c r="D235" s="4"/>
+      <c r="D235" s="6"/>
       <c r="E235" s="3"/>
       <c r="F235" s="3"/>
       <c r="G235" s="3"/>
@@ -2828,7 +3153,7 @@
       <c r="A236" s="3"/>
       <c r="B236" s="3"/>
       <c r="C236" s="3"/>
-      <c r="D236" s="4"/>
+      <c r="D236" s="6"/>
       <c r="E236" s="3"/>
       <c r="F236" s="3"/>
       <c r="G236" s="3"/>

</xml_diff>